<commit_message>
Update trainings and presenze
</commit_message>
<xml_diff>
--- a/001_2223_PGSFOGLIZZESE/U14F/trainings/000_TEMPLATE.xlsx
+++ b/001_2223_PGSFOGLIZZESE/U14F/trainings/000_TEMPLATE.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiapell/Documents/personale/CoachVolleyball/001_2223_PGSFOGLIZZESE/U14F/trainings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C2EDEBA-1C63-8E4F-9276-21427B78E752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D140DEA-3F74-B64B-8ACD-85F93E1B7E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{1BFBEE08-C1EF-1F48-9B18-291AE5124981}"/>
+    <workbookView xWindow="3260" yWindow="2140" windowWidth="28040" windowHeight="17440" xr2:uid="{1BFBEE08-C1EF-1F48-9B18-291AE5124981}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$99</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$101</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <customWorkbookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="43">
   <si>
     <t>PGS FOGLIZZESE</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Ruolo</t>
   </si>
   <si>
-    <t>Presente</t>
-  </si>
-  <si>
     <t>Obiettivo  Allenamento</t>
   </si>
   <si>
@@ -154,9 +151,6 @@
     <t>Allenamento</t>
   </si>
   <si>
-    <t>Descrizione</t>
-  </si>
-  <si>
     <t>Considerazioni generali</t>
   </si>
   <si>
@@ -167,6 +161,15 @@
   </si>
   <si>
     <t xml:space="preserve">Fase dell'anno: </t>
+  </si>
+  <si>
+    <t>Assenti</t>
+  </si>
+  <si>
+    <t>Teresa</t>
+  </si>
+  <si>
+    <t>Allenamento:</t>
   </si>
 </sst>
 </file>
@@ -445,12 +448,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -477,36 +510,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -531,13 +534,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>97366</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>726722</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>165101</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -581,7 +584,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>97366</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2280356" cy="1282700"/>
@@ -626,7 +629,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>97366</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2280356" cy="1282700"/>
@@ -671,7 +674,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>97366</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2280356" cy="1282700"/>
@@ -716,7 +719,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>97366</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2280356" cy="1282700"/>
@@ -761,7 +764,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>97366</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2280356" cy="1282700"/>
@@ -806,7 +809,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>97366</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>76</xdr:row>
       <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2280356" cy="1282700"/>
@@ -1147,10 +1150,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C5A359-32AD-8749-AF53-E139F7D1D684}">
-  <dimension ref="A1:H96"/>
+  <dimension ref="A1:H98"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1175,17 +1178,22 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G2" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
     <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
@@ -1204,1037 +1212,1057 @@
         <v>7</v>
       </c>
       <c r="F4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="25"/>
+      <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>22</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="7">
         <v>40020</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" s="5"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>42</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="D6" s="7">
         <v>40086</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="6"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>65</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="D7" s="7">
         <v>40241</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" s="6"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>11</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="D8" s="7">
         <v>39833</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" s="6"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>28</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>19</v>
       </c>
       <c r="D9" s="7">
         <v>39926</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9" s="6"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>56</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="D10" s="7">
         <v>40001</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" s="6"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>32</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="7">
         <v>39854</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" s="6"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>14</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="D12" s="7">
         <v>40143</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="6"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>27</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="D13" s="7">
         <v>40002</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F13" s="6"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>5</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="D14" s="7">
         <v>40526</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F14" s="6"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
+        <v>0</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
         <v>54</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="7">
+      <c r="B16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="7">
         <v>39921</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-    </row>
-    <row r="16" spans="1:8" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9" t="s">
+      <c r="E16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+    </row>
+    <row r="17" spans="1:8" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="9" t="s">
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:8" ht="5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:8" ht="5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A19" s="29" t="s">
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+    </row>
+    <row r="21" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+    </row>
+    <row r="22" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+    </row>
+    <row r="23" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+    </row>
+    <row r="24" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+    </row>
+    <row r="25" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+    </row>
+    <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-    </row>
-    <row r="20" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="25"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-    </row>
-    <row r="21" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="25"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-    </row>
-    <row r="22" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="25"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-    </row>
-    <row r="23" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="25"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-    </row>
-    <row r="24" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="25"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-    </row>
-    <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A26" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-    </row>
-    <row r="27" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="6"/>
-      <c r="B28" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-    </row>
-    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+    </row>
+    <row r="28" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
     </row>
     <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
     </row>
     <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-    </row>
-    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="6"/>
-      <c r="B36" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
-    </row>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+    </row>
+    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="6"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+    </row>
+    <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="6"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="25"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="6"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="25"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="6"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="25"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="25"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="6"/>
-      <c r="B44" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="25"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="6"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="6"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25"/>
-      <c r="H46" s="25"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
-      <c r="H47" s="25"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="6"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="25"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25"/>
-      <c r="H49" s="25"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="6"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="25"/>
-      <c r="G50" s="25"/>
-      <c r="H50" s="25"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="6"/>
-      <c r="B52" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="25"/>
-      <c r="G52" s="25"/>
-      <c r="H52" s="25"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="6"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="6"/>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25"/>
-      <c r="H53" s="25"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="6"/>
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="25"/>
-      <c r="G54" s="25"/>
-      <c r="H54" s="25"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="6"/>
-      <c r="B55" s="25"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="25"/>
-      <c r="H55" s="25"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="6"/>
-      <c r="B56" s="25"/>
-      <c r="C56" s="25"/>
-      <c r="D56" s="25"/>
-      <c r="E56" s="25"/>
-      <c r="F56" s="25"/>
-      <c r="G56" s="25"/>
-      <c r="H56" s="25"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="6"/>
-      <c r="B57" s="25"/>
-      <c r="C57" s="25"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="25"/>
-      <c r="F57" s="25"/>
-      <c r="G57" s="25"/>
-      <c r="H57" s="25"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="6"/>
-      <c r="B58" s="25"/>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="25"/>
-      <c r="G58" s="25"/>
-      <c r="H58" s="25"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="6"/>
-      <c r="B60" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C60" s="24"/>
-      <c r="D60" s="24"/>
-      <c r="E60" s="24"/>
-      <c r="F60" s="25"/>
-      <c r="G60" s="25"/>
-      <c r="H60" s="25"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="6"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="6"/>
-      <c r="B61" s="25"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="25"/>
-      <c r="F61" s="25"/>
-      <c r="G61" s="25"/>
-      <c r="H61" s="25"/>
+      <c r="B61" s="15"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="6"/>
-      <c r="B62" s="25"/>
-      <c r="C62" s="25"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="25"/>
-      <c r="G62" s="25"/>
-      <c r="H62" s="25"/>
+      <c r="B62" s="11"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="6"/>
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="25"/>
-      <c r="G63" s="25"/>
-      <c r="H63" s="25"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="6"/>
-      <c r="B64" s="25"/>
-      <c r="C64" s="25"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="25"/>
-      <c r="G64" s="25"/>
-      <c r="H64" s="25"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="6"/>
-      <c r="B65" s="25"/>
-      <c r="C65" s="25"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="25"/>
-      <c r="G65" s="25"/>
-      <c r="H65" s="25"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="6"/>
-      <c r="B66" s="25"/>
-      <c r="C66" s="25"/>
-      <c r="D66" s="25"/>
-      <c r="E66" s="25"/>
-      <c r="F66" s="25"/>
-      <c r="G66" s="25"/>
-      <c r="H66" s="25"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" s="6"/>
-      <c r="B68" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C68" s="24"/>
-      <c r="D68" s="24"/>
-      <c r="E68" s="24"/>
-      <c r="F68" s="25"/>
-      <c r="G68" s="25"/>
-      <c r="H68" s="25"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="6"/>
+      <c r="B67" s="11"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="11"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="6"/>
-      <c r="B69" s="25"/>
-      <c r="C69" s="25"/>
-      <c r="D69" s="25"/>
-      <c r="E69" s="25"/>
-      <c r="F69" s="25"/>
-      <c r="G69" s="25"/>
-      <c r="H69" s="25"/>
+      <c r="B69" s="15"/>
+      <c r="C69" s="15"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="15"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="11"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="6"/>
-      <c r="B70" s="25"/>
-      <c r="C70" s="25"/>
-      <c r="D70" s="25"/>
-      <c r="E70" s="25"/>
-      <c r="F70" s="25"/>
-      <c r="G70" s="25"/>
-      <c r="H70" s="25"/>
+      <c r="B70" s="11"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="11"/>
+      <c r="E70" s="11"/>
+      <c r="F70" s="11"/>
+      <c r="G70" s="11"/>
+      <c r="H70" s="11"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="6"/>
-      <c r="B71" s="25"/>
-      <c r="C71" s="25"/>
-      <c r="D71" s="25"/>
-      <c r="E71" s="25"/>
-      <c r="F71" s="25"/>
-      <c r="G71" s="25"/>
-      <c r="H71" s="25"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="11"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="6"/>
-      <c r="B72" s="25"/>
-      <c r="C72" s="25"/>
-      <c r="D72" s="25"/>
-      <c r="E72" s="25"/>
-      <c r="F72" s="25"/>
-      <c r="G72" s="25"/>
-      <c r="H72" s="25"/>
+      <c r="B72" s="11"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="11"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="11"/>
+      <c r="H72" s="11"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="6"/>
-      <c r="B73" s="25"/>
-      <c r="C73" s="25"/>
-      <c r="D73" s="25"/>
-      <c r="E73" s="25"/>
-      <c r="F73" s="25"/>
-      <c r="G73" s="25"/>
-      <c r="H73" s="25"/>
+      <c r="B73" s="11"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="11"/>
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
+      <c r="G73" s="11"/>
+      <c r="H73" s="11"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="6"/>
-      <c r="B74" s="25"/>
-      <c r="C74" s="25"/>
-      <c r="D74" s="25"/>
-      <c r="E74" s="25"/>
-      <c r="F74" s="25"/>
-      <c r="G74" s="25"/>
-      <c r="H74" s="25"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="6"/>
-      <c r="B76" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C76" s="24"/>
-      <c r="D76" s="24"/>
-      <c r="E76" s="24"/>
-      <c r="F76" s="25"/>
-      <c r="G76" s="25"/>
-      <c r="H76" s="25"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="11"/>
+      <c r="D74" s="11"/>
+      <c r="E74" s="11"/>
+      <c r="F74" s="11"/>
+      <c r="G74" s="11"/>
+      <c r="H74" s="11"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="6"/>
+      <c r="B75" s="11"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="11"/>
+      <c r="E75" s="11"/>
+      <c r="F75" s="11"/>
+      <c r="G75" s="11"/>
+      <c r="H75" s="11"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="6"/>
-      <c r="B77" s="25"/>
-      <c r="C77" s="25"/>
-      <c r="D77" s="25"/>
-      <c r="E77" s="25"/>
-      <c r="F77" s="25"/>
-      <c r="G77" s="25"/>
-      <c r="H77" s="25"/>
+      <c r="B77" s="15"/>
+      <c r="C77" s="15"/>
+      <c r="D77" s="15"/>
+      <c r="E77" s="15"/>
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="11"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="6"/>
-      <c r="B78" s="25"/>
-      <c r="C78" s="25"/>
-      <c r="D78" s="25"/>
-      <c r="E78" s="25"/>
-      <c r="F78" s="25"/>
-      <c r="G78" s="25"/>
-      <c r="H78" s="25"/>
+      <c r="B78" s="11"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="11"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="6"/>
-      <c r="B79" s="25"/>
-      <c r="C79" s="25"/>
-      <c r="D79" s="25"/>
-      <c r="E79" s="25"/>
-      <c r="F79" s="25"/>
-      <c r="G79" s="25"/>
-      <c r="H79" s="25"/>
+      <c r="B79" s="11"/>
+      <c r="C79" s="11"/>
+      <c r="D79" s="11"/>
+      <c r="E79" s="11"/>
+      <c r="F79" s="11"/>
+      <c r="G79" s="11"/>
+      <c r="H79" s="11"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="6"/>
-      <c r="B80" s="25"/>
-      <c r="C80" s="25"/>
-      <c r="D80" s="25"/>
-      <c r="E80" s="25"/>
-      <c r="F80" s="25"/>
-      <c r="G80" s="25"/>
-      <c r="H80" s="25"/>
+      <c r="B80" s="11"/>
+      <c r="C80" s="11"/>
+      <c r="D80" s="11"/>
+      <c r="E80" s="11"/>
+      <c r="F80" s="11"/>
+      <c r="G80" s="11"/>
+      <c r="H80" s="11"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="6"/>
-      <c r="B81" s="25"/>
-      <c r="C81" s="25"/>
-      <c r="D81" s="25"/>
-      <c r="E81" s="25"/>
-      <c r="F81" s="25"/>
-      <c r="G81" s="25"/>
-      <c r="H81" s="25"/>
+      <c r="B81" s="11"/>
+      <c r="C81" s="11"/>
+      <c r="D81" s="11"/>
+      <c r="E81" s="11"/>
+      <c r="F81" s="11"/>
+      <c r="G81" s="11"/>
+      <c r="H81" s="11"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="6"/>
-      <c r="B82" s="25"/>
-      <c r="C82" s="25"/>
-      <c r="D82" s="25"/>
-      <c r="E82" s="25"/>
-      <c r="F82" s="25"/>
-      <c r="G82" s="25"/>
-      <c r="H82" s="25"/>
-    </row>
-    <row r="84" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A84" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="B84" s="27"/>
-      <c r="C84" s="27"/>
-      <c r="D84" s="27"/>
-      <c r="E84" s="27"/>
-      <c r="F84" s="27"/>
-      <c r="G84" s="27"/>
-      <c r="H84" s="28"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" s="5" t="s">
+      <c r="B82" s="11"/>
+      <c r="C82" s="11"/>
+      <c r="D82" s="11"/>
+      <c r="E82" s="11"/>
+      <c r="F82" s="11"/>
+      <c r="G82" s="11"/>
+      <c r="H82" s="11"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="6"/>
+      <c r="B83" s="11"/>
+      <c r="C83" s="11"/>
+      <c r="D83" s="11"/>
+      <c r="E83" s="11"/>
+      <c r="F83" s="11"/>
+      <c r="G83" s="11"/>
+      <c r="H83" s="11"/>
+    </row>
+    <row r="85" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A85" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B85" s="21"/>
+      <c r="C85" s="21"/>
+      <c r="D85" s="21"/>
+      <c r="E85" s="21"/>
+      <c r="F85" s="21"/>
+      <c r="G85" s="21"/>
+      <c r="H85" s="22"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B86" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C85" s="5" t="s">
+      <c r="C86" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D85" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E85" s="23"/>
-      <c r="F85" s="10"/>
-      <c r="G85" s="5" t="s">
+      <c r="D86" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="H85" s="5"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="6">
-        <v>22</v>
-      </c>
-      <c r="B86" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D86" s="11"/>
-      <c r="E86" s="12"/>
-      <c r="F86" s="13"/>
-      <c r="G86" s="14"/>
-      <c r="H86" s="15"/>
+      <c r="E86" s="17"/>
+      <c r="F86" s="10"/>
+      <c r="G86" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H86" s="5"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="6">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D87" s="11"/>
-      <c r="E87" s="12"/>
-      <c r="F87" s="16"/>
-      <c r="G87" s="17"/>
-      <c r="H87" s="18"/>
+        <v>9</v>
+      </c>
+      <c r="D87" s="18"/>
+      <c r="E87" s="19"/>
+      <c r="F87" s="23"/>
+      <c r="G87" s="24"/>
+      <c r="H87" s="25"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="6">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D88" s="11"/>
-      <c r="E88" s="12"/>
-      <c r="F88" s="16"/>
-      <c r="G88" s="17"/>
-      <c r="H88" s="18"/>
+        <v>12</v>
+      </c>
+      <c r="D88" s="18"/>
+      <c r="E88" s="19"/>
+      <c r="F88" s="26"/>
+      <c r="G88" s="27"/>
+      <c r="H88" s="28"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="6">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D89" s="11"/>
-      <c r="E89" s="12"/>
-      <c r="F89" s="16"/>
-      <c r="G89" s="17"/>
-      <c r="H89" s="18"/>
+        <v>14</v>
+      </c>
+      <c r="D89" s="18"/>
+      <c r="E89" s="19"/>
+      <c r="F89" s="26"/>
+      <c r="G89" s="27"/>
+      <c r="H89" s="28"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="6">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D90" s="11"/>
-      <c r="E90" s="12"/>
-      <c r="F90" s="16"/>
-      <c r="G90" s="17"/>
-      <c r="H90" s="18"/>
+        <v>16</v>
+      </c>
+      <c r="D90" s="18"/>
+      <c r="E90" s="19"/>
+      <c r="F90" s="26"/>
+      <c r="G90" s="27"/>
+      <c r="H90" s="28"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="6">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D91" s="11"/>
-      <c r="E91" s="12"/>
-      <c r="F91" s="16"/>
-      <c r="G91" s="17"/>
-      <c r="H91" s="18"/>
+        <v>18</v>
+      </c>
+      <c r="D91" s="18"/>
+      <c r="E91" s="19"/>
+      <c r="F91" s="26"/>
+      <c r="G91" s="27"/>
+      <c r="H91" s="28"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="6">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D92" s="11"/>
-      <c r="E92" s="12"/>
-      <c r="F92" s="16"/>
-      <c r="G92" s="17"/>
-      <c r="H92" s="18"/>
+        <v>20</v>
+      </c>
+      <c r="D92" s="18"/>
+      <c r="E92" s="19"/>
+      <c r="F92" s="26"/>
+      <c r="G92" s="27"/>
+      <c r="H92" s="28"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="6">
+        <v>32</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C93" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B93" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D93" s="11"/>
-      <c r="E93" s="12"/>
-      <c r="F93" s="16"/>
-      <c r="G93" s="17"/>
-      <c r="H93" s="18"/>
+      <c r="D93" s="18"/>
+      <c r="E93" s="19"/>
+      <c r="F93" s="26"/>
+      <c r="G93" s="27"/>
+      <c r="H93" s="28"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="6">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D94" s="11"/>
-      <c r="E94" s="12"/>
-      <c r="F94" s="16"/>
-      <c r="G94" s="17"/>
-      <c r="H94" s="18"/>
+        <v>23</v>
+      </c>
+      <c r="D94" s="18"/>
+      <c r="E94" s="19"/>
+      <c r="F94" s="26"/>
+      <c r="G94" s="27"/>
+      <c r="H94" s="28"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="6">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D95" s="11"/>
-      <c r="E95" s="12"/>
-      <c r="F95" s="16"/>
-      <c r="G95" s="17"/>
-      <c r="H95" s="18"/>
+        <v>25</v>
+      </c>
+      <c r="D95" s="18"/>
+      <c r="E95" s="19"/>
+      <c r="F95" s="26"/>
+      <c r="G95" s="27"/>
+      <c r="H95" s="28"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="6">
+        <v>5</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D96" s="18"/>
+      <c r="E96" s="19"/>
+      <c r="F96" s="26"/>
+      <c r="G96" s="27"/>
+      <c r="H96" s="28"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="6">
+        <v>0</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D97" s="18"/>
+      <c r="E97" s="19"/>
+      <c r="F97" s="26"/>
+      <c r="G97" s="27"/>
+      <c r="H97" s="28"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" s="6">
         <v>54</v>
       </c>
-      <c r="B96" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D96" s="11"/>
-      <c r="E96" s="12"/>
-      <c r="F96" s="19"/>
-      <c r="G96" s="20"/>
-      <c r="H96" s="21"/>
+      <c r="B98" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D98" s="18"/>
+      <c r="E98" s="19"/>
+      <c r="F98" s="29"/>
+      <c r="G98" s="30"/>
+      <c r="H98" s="31"/>
     </row>
   </sheetData>
   <customSheetViews>
@@ -2242,98 +2270,100 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
-  <mergeCells count="91">
+  <mergeCells count="93">
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="F87:H98"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="B77:E77"/>
+    <mergeCell ref="F77:H83"/>
+    <mergeCell ref="B78:E78"/>
+    <mergeCell ref="B79:E79"/>
+    <mergeCell ref="B80:E80"/>
+    <mergeCell ref="B81:E81"/>
+    <mergeCell ref="B82:E82"/>
+    <mergeCell ref="B83:E83"/>
+    <mergeCell ref="A85:H85"/>
+    <mergeCell ref="B69:E69"/>
+    <mergeCell ref="F69:H75"/>
+    <mergeCell ref="B70:E70"/>
+    <mergeCell ref="B71:E71"/>
+    <mergeCell ref="B72:E72"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="B75:E75"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="F61:H67"/>
+    <mergeCell ref="B62:E62"/>
+    <mergeCell ref="B63:E63"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="B66:E66"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="F53:H59"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="B57:E57"/>
+    <mergeCell ref="B58:E58"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="F45:H51"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="B51:E51"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="F37:H43"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="F29:H35"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="G15:H15"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G7:H7"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="F28:H34"/>
-    <mergeCell ref="A23:H23"/>
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="F36:H42"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="F44:H50"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B50:E50"/>
-    <mergeCell ref="B52:E52"/>
-    <mergeCell ref="F52:H58"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="B57:E57"/>
-    <mergeCell ref="B58:E58"/>
-    <mergeCell ref="B60:E60"/>
-    <mergeCell ref="F60:H66"/>
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="B62:E62"/>
-    <mergeCell ref="B63:E63"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="B66:E66"/>
-    <mergeCell ref="B68:E68"/>
-    <mergeCell ref="F68:H74"/>
-    <mergeCell ref="B69:E69"/>
-    <mergeCell ref="B70:E70"/>
-    <mergeCell ref="B71:E71"/>
-    <mergeCell ref="B72:E72"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="B76:E76"/>
-    <mergeCell ref="F76:H82"/>
-    <mergeCell ref="B77:E77"/>
-    <mergeCell ref="B78:E78"/>
-    <mergeCell ref="B79:E79"/>
-    <mergeCell ref="B80:E80"/>
-    <mergeCell ref="B81:E81"/>
-    <mergeCell ref="B82:E82"/>
-    <mergeCell ref="A84:H84"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="F86:H96"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="D93:E93"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Presenze e classifica 20220920
</commit_message>
<xml_diff>
--- a/001_2223_PGSFOGLIZZESE/U14F/trainings/000_TEMPLATE.xlsx
+++ b/001_2223_PGSFOGLIZZESE/U14F/trainings/000_TEMPLATE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiapell/Documents/personale/CoachVolleyball/001_2223_PGSFOGLIZZESE/U14F/trainings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D140DEA-3F74-B64B-8ACD-85F93E1B7E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5B68C2-44FD-4143-BE1B-27F9835D0377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2140" windowWidth="28040" windowHeight="17440" xr2:uid="{1BFBEE08-C1EF-1F48-9B18-291AE5124981}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="44">
   <si>
     <t>PGS FOGLIZZESE</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>Allenamento:</t>
+  </si>
+  <si>
+    <t>N:</t>
   </si>
 </sst>
 </file>
@@ -288,51 +291,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -412,11 +370,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -439,28 +434,40 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -484,31 +491,31 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1153,7 +1160,7 @@
   <dimension ref="A1:H98"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1184,16 +1191,16 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
@@ -1214,10 +1221,10 @@
       <c r="F4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="11"/>
+      <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
@@ -1236,8 +1243,8 @@
         <v>29</v>
       </c>
       <c r="F5" s="5"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
@@ -1256,8 +1263,8 @@
         <v>29</v>
       </c>
       <c r="F6" s="6"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
@@ -1276,8 +1283,8 @@
         <v>29</v>
       </c>
       <c r="F7" s="6"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
@@ -1296,8 +1303,8 @@
         <v>29</v>
       </c>
       <c r="F8" s="6"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
@@ -1316,8 +1323,8 @@
         <v>31</v>
       </c>
       <c r="F9" s="6"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
@@ -1336,8 +1343,8 @@
         <v>30</v>
       </c>
       <c r="F10" s="6"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
@@ -1356,8 +1363,8 @@
         <v>29</v>
       </c>
       <c r="F11" s="6"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
@@ -1376,8 +1383,8 @@
         <v>29</v>
       </c>
       <c r="F12" s="6"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
@@ -1396,8 +1403,8 @@
         <v>29</v>
       </c>
       <c r="F13" s="6"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
@@ -1416,8 +1423,8 @@
         <v>29</v>
       </c>
       <c r="F14" s="6"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
@@ -1429,13 +1436,15 @@
       <c r="C15" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="D15" s="7">
+        <v>39600</v>
+      </c>
       <c r="E15" s="6" t="s">
         <v>29</v>
       </c>
       <c r="F15" s="6"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
@@ -1454,603 +1463,606 @@
         <v>30</v>
       </c>
       <c r="F16" s="6"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:8" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9" t="s">
+      <c r="B18" s="16"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="9" t="s">
+      <c r="E18" s="11"/>
+      <c r="F18" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="8"/>
+      <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:8" ht="5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
     </row>
     <row r="21" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
     </row>
     <row r="28" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
     </row>
     <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
     </row>
     <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="6"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="6"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="6"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
-      <c r="B45" s="15"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="6"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="6"/>
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="6"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="6"/>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="6"/>
-      <c r="B53" s="15"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="6"/>
-      <c r="B54" s="11"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="11"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="6"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="11"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="6"/>
-      <c r="B56" s="11"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="11"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="6"/>
-      <c r="B57" s="11"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="6"/>
-      <c r="B58" s="11"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
-      <c r="G58" s="11"/>
-      <c r="H58" s="11"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="6"/>
-      <c r="B59" s="11"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="11"/>
-      <c r="F59" s="11"/>
-      <c r="G59" s="11"/>
-      <c r="H59" s="11"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="6"/>
-      <c r="B61" s="15"/>
-      <c r="C61" s="15"/>
-      <c r="D61" s="15"/>
-      <c r="E61" s="15"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="11"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="6"/>
-      <c r="B62" s="11"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="11"/>
-      <c r="E62" s="11"/>
-      <c r="F62" s="11"/>
-      <c r="G62" s="11"/>
-      <c r="H62" s="11"/>
+      <c r="B62" s="13"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
+      <c r="H62" s="13"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="6"/>
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
-      <c r="E63" s="11"/>
-      <c r="F63" s="11"/>
-      <c r="G63" s="11"/>
-      <c r="H63" s="11"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="6"/>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
-      <c r="F64" s="11"/>
-      <c r="G64" s="11"/>
-      <c r="H64" s="11"/>
+      <c r="B64" s="13"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="6"/>
-      <c r="B65" s="11"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="11"/>
-      <c r="F65" s="11"/>
-      <c r="G65" s="11"/>
-      <c r="H65" s="11"/>
+      <c r="B65" s="13"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="6"/>
-      <c r="B66" s="11"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
-      <c r="E66" s="11"/>
-      <c r="F66" s="11"/>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11"/>
+      <c r="B66" s="13"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="6"/>
-      <c r="B67" s="11"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="11"/>
-      <c r="G67" s="11"/>
-      <c r="H67" s="11"/>
+      <c r="B67" s="13"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="6"/>
-      <c r="B69" s="15"/>
-      <c r="C69" s="15"/>
-      <c r="D69" s="15"/>
-      <c r="E69" s="15"/>
-      <c r="F69" s="11"/>
-      <c r="G69" s="11"/>
-      <c r="H69" s="11"/>
+      <c r="B69" s="17"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="13"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="6"/>
-      <c r="B70" s="11"/>
-      <c r="C70" s="11"/>
-      <c r="D70" s="11"/>
-      <c r="E70" s="11"/>
-      <c r="F70" s="11"/>
-      <c r="G70" s="11"/>
-      <c r="H70" s="11"/>
+      <c r="B70" s="13"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
+      <c r="G70" s="13"/>
+      <c r="H70" s="13"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="6"/>
-      <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
-      <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
-      <c r="G71" s="11"/>
-      <c r="H71" s="11"/>
+      <c r="B71" s="13"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="13"/>
+      <c r="H71" s="13"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="6"/>
-      <c r="B72" s="11"/>
-      <c r="C72" s="11"/>
-      <c r="D72" s="11"/>
-      <c r="E72" s="11"/>
-      <c r="F72" s="11"/>
-      <c r="G72" s="11"/>
-      <c r="H72" s="11"/>
+      <c r="B72" s="13"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="13"/>
+      <c r="H72" s="13"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="6"/>
-      <c r="B73" s="11"/>
-      <c r="C73" s="11"/>
-      <c r="D73" s="11"/>
-      <c r="E73" s="11"/>
-      <c r="F73" s="11"/>
-      <c r="G73" s="11"/>
-      <c r="H73" s="11"/>
+      <c r="B73" s="13"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="13"/>
+      <c r="G73" s="13"/>
+      <c r="H73" s="13"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="6"/>
-      <c r="B74" s="11"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="11"/>
-      <c r="F74" s="11"/>
-      <c r="G74" s="11"/>
-      <c r="H74" s="11"/>
+      <c r="B74" s="13"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="13"/>
+      <c r="G74" s="13"/>
+      <c r="H74" s="13"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="6"/>
-      <c r="B75" s="11"/>
-      <c r="C75" s="11"/>
-      <c r="D75" s="11"/>
-      <c r="E75" s="11"/>
-      <c r="F75" s="11"/>
-      <c r="G75" s="11"/>
-      <c r="H75" s="11"/>
+      <c r="B75" s="13"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="13"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="6"/>
-      <c r="B77" s="15"/>
-      <c r="C77" s="15"/>
-      <c r="D77" s="15"/>
-      <c r="E77" s="15"/>
-      <c r="F77" s="11"/>
-      <c r="G77" s="11"/>
-      <c r="H77" s="11"/>
+      <c r="B77" s="17"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="19"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="13"/>
+      <c r="G77" s="13"/>
+      <c r="H77" s="13"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="6"/>
-      <c r="B78" s="11"/>
-      <c r="C78" s="11"/>
-      <c r="D78" s="11"/>
-      <c r="E78" s="11"/>
-      <c r="F78" s="11"/>
-      <c r="G78" s="11"/>
-      <c r="H78" s="11"/>
+      <c r="B78" s="13"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="13"/>
+      <c r="E78" s="13"/>
+      <c r="F78" s="13"/>
+      <c r="G78" s="13"/>
+      <c r="H78" s="13"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="6"/>
-      <c r="B79" s="11"/>
-      <c r="C79" s="11"/>
-      <c r="D79" s="11"/>
-      <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
-      <c r="G79" s="11"/>
-      <c r="H79" s="11"/>
+      <c r="B79" s="13"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="13"/>
+      <c r="G79" s="13"/>
+      <c r="H79" s="13"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="6"/>
-      <c r="B80" s="11"/>
-      <c r="C80" s="11"/>
-      <c r="D80" s="11"/>
-      <c r="E80" s="11"/>
-      <c r="F80" s="11"/>
-      <c r="G80" s="11"/>
-      <c r="H80" s="11"/>
+      <c r="B80" s="13"/>
+      <c r="C80" s="13"/>
+      <c r="D80" s="13"/>
+      <c r="E80" s="13"/>
+      <c r="F80" s="13"/>
+      <c r="G80" s="13"/>
+      <c r="H80" s="13"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="6"/>
-      <c r="B81" s="11"/>
-      <c r="C81" s="11"/>
-      <c r="D81" s="11"/>
-      <c r="E81" s="11"/>
-      <c r="F81" s="11"/>
-      <c r="G81" s="11"/>
-      <c r="H81" s="11"/>
+      <c r="B81" s="13"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="13"/>
+      <c r="H81" s="13"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="6"/>
-      <c r="B82" s="11"/>
-      <c r="C82" s="11"/>
-      <c r="D82" s="11"/>
-      <c r="E82" s="11"/>
-      <c r="F82" s="11"/>
-      <c r="G82" s="11"/>
-      <c r="H82" s="11"/>
+      <c r="B82" s="13"/>
+      <c r="C82" s="13"/>
+      <c r="D82" s="13"/>
+      <c r="E82" s="13"/>
+      <c r="F82" s="13"/>
+      <c r="G82" s="13"/>
+      <c r="H82" s="13"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="6"/>
-      <c r="B83" s="11"/>
-      <c r="C83" s="11"/>
-      <c r="D83" s="11"/>
-      <c r="E83" s="11"/>
-      <c r="F83" s="11"/>
-      <c r="G83" s="11"/>
-      <c r="H83" s="11"/>
+      <c r="B83" s="13"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="13"/>
+      <c r="G83" s="13"/>
+      <c r="H83" s="13"/>
     </row>
     <row r="85" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A85" s="20" t="s">
+      <c r="A85" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B85" s="21"/>
-      <c r="C85" s="21"/>
-      <c r="D85" s="21"/>
-      <c r="E85" s="21"/>
-      <c r="F85" s="21"/>
-      <c r="G85" s="21"/>
-      <c r="H85" s="22"/>
+      <c r="B85" s="25"/>
+      <c r="C85" s="25"/>
+      <c r="D85" s="25"/>
+      <c r="E85" s="25"/>
+      <c r="F85" s="25"/>
+      <c r="G85" s="25"/>
+      <c r="H85" s="26"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
@@ -2062,11 +2074,11 @@
       <c r="C86" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D86" s="16" t="s">
+      <c r="D86" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E86" s="17"/>
-      <c r="F86" s="10"/>
+      <c r="E86" s="21"/>
+      <c r="F86" s="8"/>
       <c r="G86" s="5" t="s">
         <v>36</v>
       </c>
@@ -2082,11 +2094,11 @@
       <c r="C87" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D87" s="18"/>
-      <c r="E87" s="19"/>
-      <c r="F87" s="23"/>
-      <c r="G87" s="24"/>
-      <c r="H87" s="25"/>
+      <c r="D87" s="22"/>
+      <c r="E87" s="23"/>
+      <c r="F87" s="27"/>
+      <c r="G87" s="28"/>
+      <c r="H87" s="29"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="6">
@@ -2098,11 +2110,11 @@
       <c r="C88" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D88" s="18"/>
-      <c r="E88" s="19"/>
-      <c r="F88" s="26"/>
-      <c r="G88" s="27"/>
-      <c r="H88" s="28"/>
+      <c r="D88" s="22"/>
+      <c r="E88" s="23"/>
+      <c r="F88" s="30"/>
+      <c r="G88" s="31"/>
+      <c r="H88" s="32"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="6">
@@ -2114,11 +2126,11 @@
       <c r="C89" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D89" s="18"/>
-      <c r="E89" s="19"/>
-      <c r="F89" s="26"/>
-      <c r="G89" s="27"/>
-      <c r="H89" s="28"/>
+      <c r="D89" s="22"/>
+      <c r="E89" s="23"/>
+      <c r="F89" s="30"/>
+      <c r="G89" s="31"/>
+      <c r="H89" s="32"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="6">
@@ -2130,11 +2142,11 @@
       <c r="C90" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D90" s="18"/>
-      <c r="E90" s="19"/>
-      <c r="F90" s="26"/>
-      <c r="G90" s="27"/>
-      <c r="H90" s="28"/>
+      <c r="D90" s="22"/>
+      <c r="E90" s="23"/>
+      <c r="F90" s="30"/>
+      <c r="G90" s="31"/>
+      <c r="H90" s="32"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="6">
@@ -2146,11 +2158,11 @@
       <c r="C91" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D91" s="18"/>
-      <c r="E91" s="19"/>
-      <c r="F91" s="26"/>
-      <c r="G91" s="27"/>
-      <c r="H91" s="28"/>
+      <c r="D91" s="22"/>
+      <c r="E91" s="23"/>
+      <c r="F91" s="30"/>
+      <c r="G91" s="31"/>
+      <c r="H91" s="32"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="6">
@@ -2162,11 +2174,11 @@
       <c r="C92" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D92" s="18"/>
-      <c r="E92" s="19"/>
-      <c r="F92" s="26"/>
-      <c r="G92" s="27"/>
-      <c r="H92" s="28"/>
+      <c r="D92" s="22"/>
+      <c r="E92" s="23"/>
+      <c r="F92" s="30"/>
+      <c r="G92" s="31"/>
+      <c r="H92" s="32"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="6">
@@ -2178,11 +2190,11 @@
       <c r="C93" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D93" s="18"/>
-      <c r="E93" s="19"/>
-      <c r="F93" s="26"/>
-      <c r="G93" s="27"/>
-      <c r="H93" s="28"/>
+      <c r="D93" s="22"/>
+      <c r="E93" s="23"/>
+      <c r="F93" s="30"/>
+      <c r="G93" s="31"/>
+      <c r="H93" s="32"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="6">
@@ -2194,11 +2206,11 @@
       <c r="C94" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D94" s="18"/>
-      <c r="E94" s="19"/>
-      <c r="F94" s="26"/>
-      <c r="G94" s="27"/>
-      <c r="H94" s="28"/>
+      <c r="D94" s="22"/>
+      <c r="E94" s="23"/>
+      <c r="F94" s="30"/>
+      <c r="G94" s="31"/>
+      <c r="H94" s="32"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="6">
@@ -2210,11 +2222,11 @@
       <c r="C95" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D95" s="18"/>
-      <c r="E95" s="19"/>
-      <c r="F95" s="26"/>
-      <c r="G95" s="27"/>
-      <c r="H95" s="28"/>
+      <c r="D95" s="22"/>
+      <c r="E95" s="23"/>
+      <c r="F95" s="30"/>
+      <c r="G95" s="31"/>
+      <c r="H95" s="32"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="6">
@@ -2226,11 +2238,11 @@
       <c r="C96" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D96" s="18"/>
-      <c r="E96" s="19"/>
-      <c r="F96" s="26"/>
-      <c r="G96" s="27"/>
-      <c r="H96" s="28"/>
+      <c r="D96" s="22"/>
+      <c r="E96" s="23"/>
+      <c r="F96" s="30"/>
+      <c r="G96" s="31"/>
+      <c r="H96" s="32"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="6">
@@ -2242,11 +2254,11 @@
       <c r="C97" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D97" s="18"/>
-      <c r="E97" s="19"/>
-      <c r="F97" s="26"/>
-      <c r="G97" s="27"/>
-      <c r="H97" s="28"/>
+      <c r="D97" s="22"/>
+      <c r="E97" s="23"/>
+      <c r="F97" s="30"/>
+      <c r="G97" s="31"/>
+      <c r="H97" s="32"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="6">
@@ -2258,11 +2270,11 @@
       <c r="C98" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D98" s="18"/>
-      <c r="E98" s="19"/>
-      <c r="F98" s="29"/>
-      <c r="G98" s="30"/>
-      <c r="H98" s="31"/>
+      <c r="D98" s="22"/>
+      <c r="E98" s="23"/>
+      <c r="F98" s="33"/>
+      <c r="G98" s="34"/>
+      <c r="H98" s="35"/>
     </row>
   </sheetData>
   <customSheetViews>
@@ -2285,7 +2297,6 @@
     <mergeCell ref="D86:E86"/>
     <mergeCell ref="D87:E87"/>
     <mergeCell ref="D88:E88"/>
-    <mergeCell ref="B77:E77"/>
     <mergeCell ref="F77:H83"/>
     <mergeCell ref="B78:E78"/>
     <mergeCell ref="B79:E79"/>
@@ -2294,7 +2305,7 @@
     <mergeCell ref="B82:E82"/>
     <mergeCell ref="B83:E83"/>
     <mergeCell ref="A85:H85"/>
-    <mergeCell ref="B69:E69"/>
+    <mergeCell ref="B77:D77"/>
     <mergeCell ref="F69:H75"/>
     <mergeCell ref="B70:E70"/>
     <mergeCell ref="B71:E71"/>
@@ -2302,7 +2313,7 @@
     <mergeCell ref="B73:E73"/>
     <mergeCell ref="B74:E74"/>
     <mergeCell ref="B75:E75"/>
-    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="B69:D69"/>
     <mergeCell ref="F61:H67"/>
     <mergeCell ref="B62:E62"/>
     <mergeCell ref="B63:E63"/>
@@ -2310,7 +2321,7 @@
     <mergeCell ref="B65:E65"/>
     <mergeCell ref="B66:E66"/>
     <mergeCell ref="B67:E67"/>
-    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="B61:D61"/>
     <mergeCell ref="F53:H59"/>
     <mergeCell ref="B54:E54"/>
     <mergeCell ref="B55:E55"/>
@@ -2318,7 +2329,7 @@
     <mergeCell ref="B57:E57"/>
     <mergeCell ref="B58:E58"/>
     <mergeCell ref="B59:E59"/>
-    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="B53:D53"/>
     <mergeCell ref="F45:H51"/>
     <mergeCell ref="B46:E46"/>
     <mergeCell ref="B47:E47"/>
@@ -2326,7 +2337,7 @@
     <mergeCell ref="B49:E49"/>
     <mergeCell ref="B50:E50"/>
     <mergeCell ref="B51:E51"/>
-    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B45:D45"/>
     <mergeCell ref="F37:H43"/>
     <mergeCell ref="B38:E38"/>
     <mergeCell ref="B39:E39"/>
@@ -2334,17 +2345,18 @@
     <mergeCell ref="B41:E41"/>
     <mergeCell ref="B42:E42"/>
     <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B37:D37"/>
     <mergeCell ref="F29:H35"/>
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="A25:H25"/>
     <mergeCell ref="A27:H27"/>
-    <mergeCell ref="B29:E29"/>
     <mergeCell ref="B30:E30"/>
     <mergeCell ref="B31:E31"/>
     <mergeCell ref="B32:E32"/>
     <mergeCell ref="B33:E33"/>
     <mergeCell ref="B34:E34"/>
     <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B29:D29"/>
     <mergeCell ref="A23:H23"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G9:H9"/>

</xml_diff>